<commit_message>
Final Gerbers and BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Blue-Wizard-Mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\Blue-Wizard-Mod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99D6976-8A4F-44D5-BDB6-2A3E67D920EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBF56C3-6BA4-4610-9EB0-6903959095AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-9720" windowWidth="38640" windowHeight="21240" xr2:uid="{F7CA1A16-7EC5-4A0F-9C2C-0137AFA0B640}"/>
+    <workbookView xWindow="9984" yWindow="4284" windowWidth="28800" windowHeight="17628" xr2:uid="{F7CA1A16-7EC5-4A0F-9C2C-0137AFA0B640}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -188,12 +188,6 @@
     <t>Thick Film Resistors - SMD 1/4watts 470ohms 5%</t>
   </si>
   <si>
-    <t>MIC5365-3.3YD5-TR</t>
-  </si>
-  <si>
-    <t>LDO Voltage Regulators Ultra Small Single 150mA LDO</t>
-  </si>
-  <si>
     <t>C5</t>
   </si>
   <si>
@@ -294,6 +288,12 @@
   </si>
   <si>
     <t>R1, R2, R3</t>
+  </si>
+  <si>
+    <t>MIC5504-3.3YM5-TR</t>
+  </si>
+  <si>
+    <t>LDO Voltage Regulators Single 300mA LDO</t>
   </si>
 </sst>
 </file>
@@ -743,17 +743,17 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="86.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="3" max="3" width="86.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -764,9 +764,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -778,9 +778,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
@@ -792,9 +792,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>7</v>
@@ -806,9 +806,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
@@ -820,9 +820,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -834,9 +834,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -848,9 +848,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>15</v>
@@ -862,9 +862,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>17</v>
@@ -876,9 +876,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -890,9 +890,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>21</v>
@@ -904,9 +904,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>23</v>
@@ -918,9 +918,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -932,9 +932,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>27</v>
@@ -946,9 +946,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>29</v>
@@ -960,9 +960,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>31</v>
@@ -974,9 +974,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>33</v>
@@ -988,9 +988,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>35</v>
@@ -1002,9 +1002,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>37</v>
@@ -1016,9 +1016,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>39</v>
@@ -1030,9 +1030,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>41</v>
@@ -1044,9 +1044,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>43</v>
@@ -1058,9 +1058,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>45</v>
@@ -1072,9 +1072,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>47</v>
@@ -1086,9 +1086,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>49</v>
@@ -1100,36 +1100,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>82</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
@@ -1137,18 +1137,18 @@
       <c r="J28" s="6"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="10" t="s">
         <v>81</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>83</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>

</xml_diff>